<commit_message>
computing for cell values
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/employee dtr/Agote,Tony.xlsx
+++ b/exceltocsv/public/reports/employee dtr/Agote,Tony.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t>iRipple, Inc.</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>NUMBER OF TIMES TARDY</t>
+  </si>
+  <si>
+    <t>TOTAL TARDINESS</t>
   </si>
 </sst>
 </file>
@@ -271,7 +274,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -657,20 +660,29 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="0" t="str">
-        <f>SUM(F5:F19)</f>
+      <c r="B19" s="5" t="str">
+        <f>COUNT(F5:F19)</f>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="5" t="str">
+        <f>SUM(F5:F18)</f>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A20:F20"/>
   </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>

</xml_diff>

<commit_message>
fixed the formatting of excel files
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/employee dtr/Agote,Tony.xlsx
+++ b/exceltocsv/public/reports/employee dtr/Agote,Tony.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="75">
   <si>
     <t>iRipple, Inc.</t>
   </si>
@@ -1018,16 +1018,16 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="5" t="s">
+      <c r="B19" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>62</v>
       </c>
       <c r="E19" s="5" t="str">
@@ -1068,20 +1068,20 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="5" t="s">
+      <c r="B20" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>62</v>
       </c>
       <c r="E20" s="5" t="str">
-        <f>SUM(E5:E14)</f>
+        <f>SUM(E5:E15)</f>
       </c>
       <c r="F20" s="5" t="s">
         <v>62</v>
@@ -1118,22 +1118,22 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="5" t="s">
+      <c r="B21" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>62</v>
       </c>
       <c r="G21" s="5" t="str">
@@ -1168,25 +1168,25 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" s="5" t="s">
+      <c r="B22" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>62</v>
       </c>
       <c r="H22" s="5" t="str">
@@ -1219,445 +1219,445 @@
     </row>
     <row r="23"/>
     <row r="24">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C24" s="5" t="str">
         <f>FLOOR(G21/8,1)&amp;"."&amp;FLOOR(MOD(G21,8),1)&amp;"."&amp;(MOD(G21,8)-FLOOR(MOD(G21,8),1))*60</f>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="N24" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O24" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="P24" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q24" s="5" t="str">
+      <c r="D24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="L24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="N24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="O24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="P24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q24" s="0" t="str">
         <f>INT(LEFT(C25,2))</f>
       </c>
-      <c r="R24" s="5" t="str">
+      <c r="R24" s="0" t="str">
         <f>IF(LEFT(RIGHT(C25,LEN(C25)-2),1)=".",RIGHT(C25,LEN(C25)-3),RIGHT(C25,LEN(C25)-2))</f>
       </c>
-      <c r="S24" s="5" t="str">
+      <c r="S24" s="0" t="str">
         <f>INT(LEFT(R24,1))</f>
       </c>
-      <c r="T24" s="5" t="str">
+      <c r="T24" s="0" t="str">
         <f>RIGHT(R24,LEN(R24)-2)+0</f>
       </c>
-      <c r="U24" s="5" t="str">
+      <c r="U24" s="0" t="str">
         <f>Q24*8*60+S24*60+T24</f>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C25" s="5" t="str">
         <f>FLOOR(E20/8,1)&amp;"."&amp;FLOOR(MOD(E20,8),1)&amp;"."&amp;(MOD(E20,8)-FLOOR(MOD(E20,8),1))*60</f>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="M25" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="N25" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O25" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="P25" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q25" s="5" t="str">
+      <c r="D25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="L25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="N25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="O25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="P25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q25" s="0" t="str">
         <f>INT(LEFT(C26,2))</f>
       </c>
-      <c r="R25" s="5" t="str">
+      <c r="R25" s="0" t="str">
         <f>IF(LEFT(RIGHT(C26,LEN(C26)-2),1)=".",RIGHT(C26,LEN(C26)-3),RIGHT(C26,LEN(C26)-2))</f>
       </c>
-      <c r="S25" s="5" t="str">
+      <c r="S25" s="0" t="str">
         <f>INT(LEFT(R25,1))</f>
       </c>
-      <c r="T25" s="5" t="str">
+      <c r="T25" s="0" t="str">
         <f>RIGHT(R25,LEN(R25)-2)+0</f>
       </c>
-      <c r="U25" s="5" t="str">
+      <c r="U25" s="0" t="str">
         <f>Q25*8*60+S25*60+T25</f>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C26" s="5" t="str">
         <f>FLOOR(H22,1)&amp;"."&amp;(H22-FLOOR(H22,1))*8&amp;".0"</f>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="N26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="P26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q26" s="5" t="str">
+      <c r="D26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="K26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="L26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="M26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="N26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="O26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="P26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q26" s="0" t="str">
         <f>INT(LEFT(C27,2))</f>
       </c>
-      <c r="R26" s="5" t="str">
+      <c r="R26" s="0" t="str">
         <f>IF(LEFT(RIGHT(C27,LEN(C27)-2),1)=".",RIGHT(C27,LEN(C27)-3),RIGHT(C27,LEN(C27)-2))</f>
       </c>
-      <c r="S26" s="5" t="str">
+      <c r="S26" s="0" t="str">
         <f>INT(LEFT(R26,1))</f>
       </c>
-      <c r="T26" s="5" t="str">
+      <c r="T26" s="0" t="str">
         <f>RIGHT(R26,LEN(R26)-2)+0</f>
       </c>
-      <c r="U26" s="5" t="str">
+      <c r="U26" s="0" t="str">
         <f>Q26*8*60+S26*60+T26</f>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C27" s="5" t="str">
         <f>FLOOR(I22,1)&amp;"."&amp;(I22-FLOOR(I22,1))*8&amp;".0"</f>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="N27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="P27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q27" s="5" t="str">
+      <c r="D27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="N27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="O27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="P27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q27" s="0" t="str">
         <f>INT(LEFT(C28,2))</f>
       </c>
-      <c r="R27" s="5" t="str">
+      <c r="R27" s="0" t="str">
         <f>IF(LEFT(RIGHT(C28,LEN(C28)-2),1)=".",RIGHT(C28,LEN(C28)-3),RIGHT(C28,LEN(C28)-2))</f>
       </c>
-      <c r="S27" s="5" t="str">
+      <c r="S27" s="0" t="str">
         <f>INT(LEFT(R27,1))</f>
       </c>
-      <c r="T27" s="5" t="str">
+      <c r="T27" s="0" t="str">
         <f>RIGHT(R27,LEN(R27)-2)+0</f>
       </c>
-      <c r="U27" s="5" t="str">
+      <c r="U27" s="0" t="str">
         <f>Q27*8*60+S27*60+T27</f>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="N28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="P28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q28" s="5" t="str">
+      <c r="D28" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="M28" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="N28" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="O28" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="P28" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q28" s="0" t="str">
         <f>INT(LEFT(C29,2))</f>
       </c>
-      <c r="R28" s="5" t="str">
+      <c r="R28" s="0" t="str">
         <f>IF(LEFT(RIGHT(C29,LEN(C29)-2),1)=".",RIGHT(C29,LEN(C29)-3),RIGHT(C29,LEN(C29)-2))</f>
       </c>
-      <c r="S28" s="5" t="str">
+      <c r="S28" s="0" t="str">
         <f>INT(LEFT(R28,1))</f>
       </c>
-      <c r="T28" s="5" t="str">
+      <c r="T28" s="0" t="str">
         <f>RIGHT(R28,LEN(R28)-2)+0</f>
       </c>
-      <c r="U28" s="5" t="str">
+      <c r="U28" s="0" t="str">
         <f>Q28*8*60+S28*60+T28</f>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="M29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="N29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="P29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q29" s="5" t="str">
+      <c r="D29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="K29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="L29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="M29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="N29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="O29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="P29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q29" s="0" t="str">
         <f>Q24+IF(Q25&gt;Q27,Q25-Q27,0)+IF(Q26&gt;Q28,Q26-Q28,0)</f>
       </c>
-      <c r="R29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="S29" s="5" t="str">
+      <c r="R29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="S29" s="0" t="str">
         <f>S24+IF(S25&gt;S27,S25-S27,0)+IF(S26&gt;S28,S26-S28,0)</f>
       </c>
-      <c r="T29" s="5" t="str">
+      <c r="T29" s="0" t="str">
         <f>T24+IF(T25&gt;T27,T25-T27,0)+IF(T26&gt;T28,T26-T28,0)</f>
       </c>
-      <c r="U29" s="5" t="str">
+      <c r="U29" s="0" t="str">
         <f>U24+IF(U25&gt;U27,U25-U27,0)+IF(U26&gt;U28,U26-U28,0)</f>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="9" t="s">
         <v>62</v>
       </c>
       <c r="C30" s="5" t="str">
         <f>FLOOR(Q30/8,1)&amp;"."&amp;FLOOR(MOD(Q30,8),1)&amp;"."&amp;(MOD(Q30,8)-FLOOR(MOD(Q30,8),1))*60</f>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="N30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="P30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q30" s="5" t="str">
+      <c r="D30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="K30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="L30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="M30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="N30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="O30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="P30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q30" s="0" t="str">
         <f>U29/60</f>
       </c>
     </row>
@@ -1668,13 +1668,13 @@
     <mergeCell ref="A2:P2"/>
     <mergeCell ref="A3:P3"/>
     <mergeCell ref="A19:D19"/>
-    <mergeCell ref="F19:O19"/>
+    <mergeCell ref="F19:P19"/>
     <mergeCell ref="A20:D20"/>
-    <mergeCell ref="F20:O20"/>
+    <mergeCell ref="F20:P20"/>
     <mergeCell ref="A21:F21"/>
-    <mergeCell ref="H21:O21"/>
+    <mergeCell ref="H21:P21"/>
     <mergeCell ref="A22:G22"/>
-    <mergeCell ref="J22:O22"/>
+    <mergeCell ref="J22:P22"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A26:B26"/>

</xml_diff>